<commit_message>
Added improvements after presentation
</commit_message>
<xml_diff>
--- a/Thesis/files/Data All Users Combined - More Stations.xlsx
+++ b/Thesis/files/Data All Users Combined - More Stations.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17750" tabRatio="844"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17750" tabRatio="844" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="All Data" sheetId="2" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="30">
   <si>
     <t>Precision</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Mean</t>
   </si>
 </sst>
 </file>
@@ -1561,6 +1564,61 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Users sorted by F-Measure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3849,6 +3907,61 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Users sorted by F-Measure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6137,6 +6250,61 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Users sorted by F-Measure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8425,6 +8593,61 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Users sorted by F-Measure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -10713,6 +10936,61 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Users sorted by F-Measure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -13001,6 +13279,61 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Users sorted by F-Measure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -15289,6 +15622,61 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Users sorted by F-Measure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -24937,8 +25325,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H1843"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45187,7 +45575,7 @@
   <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="G4:J9"/>
+      <selection activeCell="G10" sqref="G10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45403,6 +45791,21 @@
       <c r="E10" s="2">
         <v>1</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="2">
+        <f>HARMEAN(C4:C217)</f>
+        <v>0.85153533982029939</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" ref="I10:J10" si="0">HARMEAN(D4:D217)</f>
+        <v>0.91377200426359917</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.88148893881713353</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
@@ -47924,8 +48327,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J217"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -48141,6 +48544,21 @@
       <c r="E10" s="2">
         <v>1</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="2">
+        <f>HARMEAN(C4:C217)</f>
+        <v>0.85406214961618265</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" ref="I10:J10" si="0">HARMEAN(D4:D217)</f>
+        <v>0.88345733471840082</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.86833697103413032</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
@@ -50660,7 +51078,7 @@
   <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J9"/>
+      <selection activeCell="G10" sqref="G10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -50878,6 +51296,21 @@
       <c r="E10" s="2">
         <v>1</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="2">
+        <f>HARMEAN(C4:C217)</f>
+        <v>0.85550143835390313</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" ref="I10:J10" si="0">HARMEAN(D4:D217)</f>
+        <v>0.8800665338286735</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.86739961446842428</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
@@ -53397,7 +53830,7 @@
   <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53613,6 +54046,21 @@
       <c r="E10" s="2">
         <v>1</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="2">
+        <f>HARMEAN(C4:C217)</f>
+        <v>0.84655686296744326</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" ref="I10:J10" si="0">HARMEAN(D4:D217)</f>
+        <v>0.90855137591793411</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.87633334484595238</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
@@ -56132,7 +56580,7 @@
   <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J9"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -56348,6 +56796,21 @@
       <c r="E10" s="2">
         <v>1</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="2">
+        <f>HARMEAN(C4:C217)</f>
+        <v>0.8474970500600526</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" ref="I10:J10" si="0">HARMEAN(D4:D217)</f>
+        <v>0.91775527052735106</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.88117059134255382</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
@@ -58867,7 +59330,7 @@
   <dimension ref="A1:J651"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -59085,6 +59548,21 @@
       <c r="E10" s="2">
         <v>1</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="2">
+        <f>HARMEAN(C4:C217)</f>
+        <v>0.84909316389736722</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" ref="I10:J10" si="0">HARMEAN(D4:D217)</f>
+        <v>0.91592210397742602</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.88099276024215611</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>

</xml_diff>